<commit_message>
Read the excel file using Apache POI class adding by alam
</commit_message>
<xml_diff>
--- a/CucumberBDD/TestData/testData.xlsx
+++ b/CucumberBDD/TestData/testData.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedalam/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedalam/git/repository3/CucumberBDD/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E29117F-BFFF-E246-9A7A-4CE01621A2D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F438CC99-B9D8-C24C-858E-DF4CD056FC64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14120" xr2:uid="{1171DB83-58B8-7B44-ADCF-FDA67810F78E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -402,7 +405,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,4 +437,40 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{299B24CE-8846-3849-89F6-FE9F5C304190}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956B32CC-0640-AA4B-A0E8-9E7E1883F1E6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D29DD50-D53B-0C43-AD84-235B42137484}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>